<commit_message>
added vectors to EPSSprep.xlsx + typo fix in vectors.md
</commit_message>
<xml_diff>
--- a/src/EPSSprep.xlsx
+++ b/src/EPSSprep.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Komputer\cvss_converter\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anecz\Documents\GitHub\cvss_converter\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C43DD2-C1EE-4D30-9607-449EC3411B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC14C67-C4C8-499A-868B-0B51CFFED944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{0782FCE9-53B5-476A-BEC6-6CF2CEA596EF}"/>
+    <workbookView xWindow="5085" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{0782FCE9-53B5-476A-BEC6-6CF2CEA596EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>CVE</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Base Score 4.0</t>
   </si>
   <si>
-    <t>qqqqqqqqqqqqqqqqqqqqqqqqqqqq</t>
-  </si>
-  <si>
     <t>CVE-2014-6271</t>
   </si>
   <si>
@@ -116,21 +113,9 @@
     <t>CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:C/C:H/I:H/A:H</t>
   </si>
   <si>
-    <t>9.8.</t>
-  </si>
-  <si>
-    <t>10.0.</t>
-  </si>
-  <si>
     <t>AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:H/CR:H/IR:H/AR:H/S:N/AU:Y/V:C</t>
   </si>
   <si>
-    <t>9.3.</t>
-  </si>
-  <si>
-    <t>8.9.</t>
-  </si>
-  <si>
     <t>AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:H/CR:H/IR:H/AR:H/S:P/AU:Y/V:C</t>
   </si>
   <si>
@@ -147,13 +132,25 @@
   </si>
   <si>
     <t> CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:U/C:H/I:H/A:H</t>
+  </si>
+  <si>
+    <t>CVSS:3.1/AV:L/AC:L/PR:N/UI:R/S:U/C:H/I:H/A:H</t>
+  </si>
+  <si>
+    <t>CVSS:4.0/AV:L/AC:L/AT:N/PR:N/UI:P/VC:H/VI:H/VA:H/SC:N/SI:N/SA:N/E:P/CR:H/IR:H/AR:H/S:P/AU:Y/V:C/U:Amber</t>
+  </si>
+  <si>
+    <t>CVSS:4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:H/SC:N/SI:N/SA:N/E:P/CR:H/IR:H/AR:H/S:P/AU:Y/V:C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +160,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,14 +189,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,23 +548,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4A9108-357F-4335-B5CD-24E4C445DFC3}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
-    <col min="3" max="3" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="101.36328125" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="101.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -570,148 +578,193 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>9.8000000000000007</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>9.8000000000000007</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>9.8000000000000007</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>9.8000000000000007</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -719,108 +772,108 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>8.9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>8.9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F13">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>9.8000000000000007</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F14">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to jupyter & excel
x Reduced the redundant spaces in the excel file
x Added EPSS score overview
x Added >,<,== for the comparison of scores
</commit_message>
<xml_diff>
--- a/src/EPSSprep.xlsx
+++ b/src/EPSSprep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Komputer\cvss_converter\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zycho\Documents\GitHub\cvss_converter\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A45C0F-910C-48AC-91FF-644551DB8126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82304DB-342E-428E-A037-15E2E6571810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{0782FCE9-53B5-476A-BEC6-6CF2CEA596EF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{0782FCE9-53B5-476A-BEC6-6CF2CEA596EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>CVE</t>
   </si>
@@ -92,18 +92,12 @@
     <t>CVE-2023-27350</t>
   </si>
   <si>
-    <t xml:space="preserve"> CVE-2023-27532</t>
-  </si>
-  <si>
     <t>CVE-2023-4863</t>
   </si>
   <si>
     <t>CVE-2023-5217</t>
   </si>
   <si>
-    <t xml:space="preserve"> CVE-2021-27877</t>
-  </si>
-  <si>
     <t>Vector 4.0 (with all the additional metrics)</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>CVSS:4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:H/SC:N/SI:N/SA:N/E:A/CR:H/IR:H/AR:H/S:P/AU:Y/R:I/V:C/RE:M/U:Red</t>
   </si>
   <si>
-    <t> CVSS:3.1/AV:N/AC:L/PR:N/UI:N/S:U/C:H/I:H/A:H</t>
-  </si>
-  <si>
     <t>CVSS:3.1/AV:L/AC:L/PR:N/UI:R/S:U/C:H/I:H/A:H</t>
   </si>
   <si>
@@ -153,6 +144,12 @@
   </si>
   <si>
     <t>CVSS:4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:H/SC:N/SI:N/SA:N/E:A/CR:H/IR:H/AR:H/S:P/AU:Y/R:I/V:C/RE:M/U:Amber</t>
+  </si>
+  <si>
+    <t>CVE-2021-27877</t>
+  </si>
+  <si>
+    <t>CVE-2023-27532</t>
   </si>
 </sst>
 </file>
@@ -562,7 +559,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -603,13 +600,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>9.8000000000000007</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>9.3000000000000007</v>
@@ -623,13 +620,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>9.8000000000000007</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F3">
         <v>8.9</v>
@@ -643,13 +640,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>9.8000000000000007</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>8.9</v>
@@ -663,13 +660,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>9.8000000000000007</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5">
         <v>8.9</v>
@@ -683,13 +680,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -703,13 +700,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2">
         <v>7.8</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1">
         <v>7.1</v>
@@ -723,13 +720,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1">
         <v>8.9</v>
@@ -743,13 +740,13 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1">
         <v>8.9</v>
@@ -763,13 +760,13 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1">
         <v>8.9</v>
@@ -783,13 +780,13 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11">
         <v>8.9</v>
@@ -800,16 +797,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>8.9</v>
@@ -823,13 +820,13 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13">
         <v>9.3000000000000007</v>
@@ -843,13 +840,13 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>9.8000000000000007</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14">
         <v>9.3000000000000007</v>
@@ -863,13 +860,13 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>9.8000000000000007</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15">
         <v>9.3000000000000007</v>
@@ -880,16 +877,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>7.5</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F16">
         <v>7.6</v>
@@ -900,16 +897,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>8.8000000000000007</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F17">
         <v>9.3000000000000007</v>
@@ -920,16 +917,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>8.8000000000000007</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F18">
         <v>9.3000000000000007</v>

</xml_diff>